<commit_message>
Re-implement unit tests for /todos and /todos/:id
</commit_message>
<xml_diff>
--- a/ExploratorySessionNotes/TodoSessionFiles/TodoSession.xlsx
+++ b/ExploratorySessionNotes/TodoSessionFiles/TodoSession.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\git\ecse429-project-partA\ExploratorySessionNotes\TodoSessionFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4D4599-0081-4744-9F8A-6D44BBB994BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C9441B-CABA-4F08-B9C7-6FDD95721C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="157">
   <si>
     <t>Method</t>
   </si>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t>id was not included in body. Content-Type: application/xml</t>
-  </si>
-  <si>
-    <t>bug?</t>
   </si>
   <si>
     <t>return error message mentioning invalid body format</t>
@@ -1137,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="34" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="15" customHeight="1"/>
@@ -1227,7 +1224,7 @@
         <v>56</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>27</v>
@@ -1253,7 +1250,7 @@
         <v>56</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>28</v>
@@ -1334,9 +1331,6 @@
       <c r="H7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="I7" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="8" spans="1:9" ht="31">
       <c r="A8" s="24" t="s">
@@ -1429,16 +1423,16 @@
         <v>5</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>62</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>37</v>
@@ -1456,7 +1450,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>6</v>
@@ -1479,7 +1473,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>6</v>
@@ -1502,7 +1496,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>6</v>
@@ -1527,7 +1521,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>6</v>
@@ -1543,7 +1537,7 @@
     </row>
     <row r="16" spans="1:9" ht="15.5">
       <c r="A16" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>4</v>
@@ -1552,7 +1546,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>6</v>
@@ -1562,7 +1556,7 @@
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I16" s="6"/>
     </row>
@@ -1577,7 +1571,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>6</v>
@@ -1591,7 +1585,7 @@
     </row>
     <row r="18" spans="1:9" ht="15.5">
       <c r="A18" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>4</v>
@@ -1600,7 +1594,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>6</v>
@@ -1609,16 +1603,16 @@
         <v>56</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" ht="15.5">
       <c r="A19" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>26</v>
@@ -1627,7 +1621,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>6</v>
@@ -1636,16 +1630,16 @@
         <v>56</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" ht="15.5">
       <c r="A20" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>26</v>
@@ -1654,7 +1648,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>6</v>
@@ -1664,13 +1658,13 @@
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9" ht="31">
       <c r="A21" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>9</v>
@@ -1679,7 +1673,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>62</v>
@@ -1695,7 +1689,7 @@
     </row>
     <row r="22" spans="1:9" ht="15.5">
       <c r="A22" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>9</v>
@@ -1704,7 +1698,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>6</v>
@@ -1716,13 +1710,13 @@
         <v>65</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9" ht="15.5">
       <c r="A23" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>9</v>
@@ -1731,7 +1725,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>6</v>
@@ -1747,7 +1741,7 @@
     </row>
     <row r="24" spans="1:9" ht="31">
       <c r="A24" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>9</v>
@@ -1756,7 +1750,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>6</v>
@@ -1765,16 +1759,16 @@
         <v>56</v>
       </c>
       <c r="G24" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="13" t="s">
         <v>93</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>94</v>
       </c>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9" ht="31">
       <c r="A25" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>7</v>
@@ -1783,7 +1777,7 @@
         <v>5</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>62</v>
@@ -1795,13 +1789,13 @@
         <v>64</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9" ht="15.5">
       <c r="A26" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>7</v>
@@ -1810,7 +1804,7 @@
         <v>5</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>6</v>
@@ -1822,13 +1816,13 @@
         <v>65</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" ht="31">
       <c r="A27" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>7</v>
@@ -1837,7 +1831,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>6</v>
@@ -1846,16 +1840,16 @@
         <v>56</v>
       </c>
       <c r="G27" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H27" s="13" t="s">
         <v>98</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>99</v>
       </c>
       <c r="I27" s="7"/>
     </row>
     <row r="28" spans="1:9" ht="46.5">
       <c r="A28" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>7</v>
@@ -1864,7 +1858,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>6</v>
@@ -1873,7 +1867,7 @@
         <v>56</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H28" s="13"/>
       <c r="I28" s="7"/>
@@ -1889,7 +1883,7 @@
         <v>5</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>6</v>
@@ -1921,16 +1915,16 @@
         <v>56</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9" ht="15.5">
       <c r="A31" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>10</v>
@@ -1939,7 +1933,7 @@
         <v>5</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>6</v>
@@ -1949,13 +1943,13 @@
       </c>
       <c r="G31" s="16"/>
       <c r="H31" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:9" ht="15.5">
       <c r="A32" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>10</v>
@@ -1964,7 +1958,7 @@
         <v>5</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>6</v>
@@ -1974,13 +1968,13 @@
       </c>
       <c r="G32" s="16"/>
       <c r="H32" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:9" ht="15.5">
       <c r="A33" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>26</v>
@@ -1989,7 +1983,7 @@
         <v>5</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>6</v>
@@ -1999,13 +1993,13 @@
       </c>
       <c r="G33" s="16"/>
       <c r="H33" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I33" s="7"/>
     </row>
     <row r="34" spans="1:9" ht="31">
       <c r="A34" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>11</v>
@@ -2014,7 +2008,7 @@
         <v>5</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>6</v>
@@ -2024,13 +2018,13 @@
       </c>
       <c r="G34" s="16"/>
       <c r="H34" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:9" ht="31">
       <c r="A35" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>11</v>
@@ -2039,7 +2033,7 @@
         <v>5</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>6</v>
@@ -2049,13 +2043,13 @@
       </c>
       <c r="G35" s="16"/>
       <c r="H35" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I35" s="7"/>
     </row>
     <row r="36" spans="1:9" ht="15.5">
       <c r="A36" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>12</v>
@@ -2064,7 +2058,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>6</v>
@@ -2074,7 +2068,7 @@
       </c>
       <c r="G36" s="16"/>
       <c r="H36" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I36" s="7"/>
     </row>
@@ -2098,10 +2092,10 @@
         <v>56</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I37" s="7"/>
     </row>
@@ -2116,7 +2110,7 @@
         <v>5</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>6</v>
@@ -2125,16 +2119,16 @@
         <v>56</v>
       </c>
       <c r="G38" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38" s="13" t="s">
         <v>116</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>117</v>
       </c>
       <c r="I38" s="7"/>
     </row>
     <row r="39" spans="1:9" ht="15.5">
       <c r="A39" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>4</v>
@@ -2143,7 +2137,7 @@
         <v>5</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E39" s="9" t="s">
         <v>6</v>
@@ -2153,13 +2147,13 @@
       </c>
       <c r="G39" s="16"/>
       <c r="H39" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I39" s="6"/>
     </row>
     <row r="40" spans="1:9" ht="15.5">
       <c r="A40" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>4</v>
@@ -2168,7 +2162,7 @@
         <v>5</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>6</v>
@@ -2178,13 +2172,13 @@
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:9" ht="15.5">
       <c r="A41" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>4</v>
@@ -2193,7 +2187,7 @@
         <v>5</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>6</v>
@@ -2203,13 +2197,13 @@
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:9" ht="46.5">
       <c r="A42" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>4</v>
@@ -2218,7 +2212,7 @@
         <v>5</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E42" s="9" t="s">
         <v>6</v>
@@ -2232,7 +2226,7 @@
     </row>
     <row r="43" spans="1:9" ht="15.5">
       <c r="A43" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>4</v>
@@ -2241,7 +2235,7 @@
         <v>5</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E43" s="9" t="s">
         <v>6</v>
@@ -2251,13 +2245,13 @@
       </c>
       <c r="G43" s="16"/>
       <c r="H43" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I43" s="7"/>
     </row>
     <row r="44" spans="1:9" ht="15.5">
       <c r="A44" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>4</v>
@@ -2266,7 +2260,7 @@
         <v>5</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E44" s="9" t="s">
         <v>6</v>
@@ -2276,13 +2270,13 @@
       </c>
       <c r="G44" s="16"/>
       <c r="H44" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I44" s="7"/>
     </row>
     <row r="45" spans="1:9" ht="15.5">
       <c r="A45" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>4</v>
@@ -2291,7 +2285,7 @@
         <v>5</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E45" s="9" t="s">
         <v>6</v>
@@ -2305,7 +2299,7 @@
     </row>
     <row r="46" spans="1:9" ht="31">
       <c r="A46" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>4</v>
@@ -2314,7 +2308,7 @@
         <v>5</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>6</v>
@@ -2324,13 +2318,13 @@
       </c>
       <c r="G46" s="16"/>
       <c r="H46" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="1:9" ht="31">
       <c r="A47" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>4</v>
@@ -2339,7 +2333,7 @@
         <v>5</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E47" s="9" t="s">
         <v>6</v>
@@ -2349,13 +2343,13 @@
       </c>
       <c r="G47" s="16"/>
       <c r="H47" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="1:9" ht="31">
       <c r="A48" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>4</v>
@@ -2364,23 +2358,23 @@
         <v>8</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E48" s="9" t="s">
         <v>62</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G48" s="16"/>
       <c r="H48" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I48" s="7"/>
     </row>
     <row r="49" spans="1:9" ht="46.5">
       <c r="A49" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>4</v>
@@ -2389,7 +2383,7 @@
         <v>5</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E49" s="9" t="s">
         <v>6</v>
@@ -2399,7 +2393,7 @@
       </c>
       <c r="G49" s="16"/>
       <c r="H49" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I49" s="7"/>
     </row>
@@ -4666,7 +4660,7 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -4737,7 +4731,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -4856,7 +4850,7 @@
     <row r="15" spans="1:8" ht="31">
       <c r="A15" s="3"/>
       <c r="B15" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -4867,7 +4861,7 @@
     </row>
     <row r="16" spans="1:8" ht="31">
       <c r="B16" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -4891,7 +4885,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -4903,7 +4897,7 @@
     <row r="19" spans="1:8" ht="46.5">
       <c r="A19" s="3"/>
       <c r="B19" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -4914,7 +4908,7 @@
     </row>
     <row r="20" spans="1:8" ht="15.5">
       <c r="B20" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -4960,7 +4954,7 @@
     <row r="24" spans="1:8" ht="15.5">
       <c r="A24" s="3"/>
       <c r="B24" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>

</xml_diff>